<commit_message>
made changes to spreadsheets
</commit_message>
<xml_diff>
--- a/kinetic parameter error vs kinetic parameter.xlsx
+++ b/kinetic parameter error vs kinetic parameter.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\Documents\bioreactor-kinetic-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5312E476-9B66-4353-A61C-8D12831876BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9290FE-04EC-4157-A871-785F338C6C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F29D0799-2F30-4BDD-A825-225B754274AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F29D0799-2F30-4BDD-A825-225B754274AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="48">
   <si>
     <t>R1P</t>
   </si>
@@ -106,12 +109,84 @@
   <si>
     <t>Gamma Error</t>
   </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +204,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,12 +235,32 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -166,11 +269,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -248,6 +359,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$6</c:f>
@@ -1933,6 +2088,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.405336832895888E-2"/>
+                  <c:y val="-0.62050925925925926"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$76:$A$80</c:f>
@@ -6686,6 +6891,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$G$2:$G$6</c:f>
@@ -23627,11 +23876,693 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEAAB72-F66E-4E81-AE31-EAFBC7F6405C}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.999708432352302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.99941694971629724</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.99922259962172966</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4">
+        <v>9.0673406918379852E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4.2278719212119967E-3</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4.2278719212119967E-3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5142.3538122788677</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5.9761826475755783E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.4665000166558285E-6</v>
+      </c>
+      <c r="D13" s="4">
+        <v>8.2216667221860952E-7</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="5">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>4.2303384212286528E-3</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1.0152233404995108</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.4055840470570258E-2</v>
+      </c>
+      <c r="D17" s="4">
+        <v>72.227864468521688</v>
+      </c>
+      <c r="E17" s="4">
+        <v>5.8486658602051351E-6</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.97049138292628723</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1.0599552980727343</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.97049138292628723</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1.0599552980727343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-49.286609704220403</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.68730257029921071</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-71.710207169404214</v>
+      </c>
+      <c r="E18" s="5">
+        <v>5.9761826475755673E-6</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-51.473913229681123</v>
+      </c>
+      <c r="G18" s="5">
+        <v>-47.099306178759683</v>
+      </c>
+      <c r="H18" s="5">
+        <v>-51.473913229681123</v>
+      </c>
+      <c r="I18" s="5">
+        <v>-47.099306178759683</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902F50DA-5891-4DAC-A7F9-F7DC53BDFF9E}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.68772326380811388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.47296328758288458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.29728438344384611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.8018614883495723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>8.7407887390697407</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8.7407887390697407</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2.6922030843758269</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.19937631784363111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>9.7401144695920063</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3.2467048231973354</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="5">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>18.480903208661747</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2.6370160576301784</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.3980459819253368</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.8862155406352072</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.15573544618952889</v>
+      </c>
+      <c r="F17" s="4">
+        <v>-1.8121902121648445</v>
+      </c>
+      <c r="G17" s="4">
+        <v>7.086222327425201</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-1.8121902121648445</v>
+      </c>
+      <c r="I17" s="4">
+        <v>7.086222327425201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-46.804598470019208</v>
+      </c>
+      <c r="C18" s="5">
+        <v>28.525588642431032</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-1.6407934313544243</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.19937631784363113</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-137.58575265116679</v>
+      </c>
+      <c r="G18" s="5">
+        <v>43.976555711128363</v>
+      </c>
+      <c r="H18" s="5">
+        <v>-137.58575265116679</v>
+      </c>
+      <c r="I18" s="5">
+        <v>43.976555711128363</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E6E553-D8D7-4DBD-B527-CFD4693794BD}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.99987001850544299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.9997400539060749</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.99965340520809987</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4.1227859432857379E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.9611310882810722E-3</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.9611310882810722E-3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>11537.854315988252</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1.7788842055957064E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5.099209180246341E-7</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.699736393415447E-7</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="5">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1.9616410091990969E-3</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1.0555260014165646</v>
+      </c>
+      <c r="C17" s="4">
+        <v>9.5712231592916339E-3</v>
+      </c>
+      <c r="D17" s="4">
+        <v>110.281202710426</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.6437574191212446E-6</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1.0250660976362311</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1.0859859051968981</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1.0250660976362311</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1.0859859051968981</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-37.695792148875292</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.3509379611474952</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-107.41440460193527</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1.7788842055957064E-6</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-38.812633366712937</v>
+      </c>
+      <c r="G18" s="5">
+        <v>-36.578950931037646</v>
+      </c>
+      <c r="H18" s="5">
+        <v>-38.812633366712937</v>
+      </c>
+      <c r="I18" s="5">
+        <v>-36.578950931037646</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D775691-4A38-415E-B0CA-C8A179265517}">
-  <dimension ref="A1:X80"/>
+  <dimension ref="A1:X82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q144" sqref="Q144"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P76" sqref="P76:P80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24337,7 +25268,7 @@
         <v>5.9412690035705407E-6</v>
       </c>
       <c r="U77">
-        <f t="shared" ref="U77:V77" si="17">U3</f>
+        <f t="shared" ref="U77" si="17">U3</f>
         <v>12</v>
       </c>
       <c r="V77">
@@ -24435,7 +25366,7 @@
         <v>4.809009990871309E-6</v>
       </c>
       <c r="U78">
-        <f t="shared" ref="U78:V78" si="35">U4</f>
+        <f t="shared" ref="U78" si="35">U4</f>
         <v>14</v>
       </c>
       <c r="V78">
@@ -24533,7 +25464,7 @@
         <v>-1.3086422792485809E-6</v>
       </c>
       <c r="U79">
-        <f t="shared" ref="U79:V79" si="53">U5</f>
+        <f t="shared" ref="U79" si="53">U5</f>
         <v>16</v>
       </c>
       <c r="V79">
@@ -24631,7 +25562,7 @@
         <v>-1.1029945546914275E-6</v>
       </c>
       <c r="U80">
-        <f t="shared" ref="U80:V80" si="71">U6</f>
+        <f t="shared" ref="U80" si="71">U6</f>
         <v>18</v>
       </c>
       <c r="V80">
@@ -24645,6 +25576,56 @@
       <c r="X80">
         <f t="shared" ref="X80" si="73">X6/W6</f>
         <v>-4.5641234572505921E-4</v>
+      </c>
+    </row>
+    <row r="82" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <f>PEARSON(A77:A80,B77:B80)</f>
+        <v>-0.99983685378612741</v>
+      </c>
+      <c r="D82">
+        <f>PEARSON(C77:C80,D77:D80)</f>
+        <v>0.91641803234003116</v>
+      </c>
+      <c r="F82">
+        <f>PEARSON(E77:E80,F77:F80)</f>
+        <v>-0.93624768793357616</v>
+      </c>
+      <c r="H82">
+        <f>PEARSON(G77:G80,H77:H80)</f>
+        <v>-0.97953397878284987</v>
+      </c>
+      <c r="J82">
+        <f>PEARSON(I77:I80,J77:J80)</f>
+        <v>-0.92873102560685095</v>
+      </c>
+      <c r="L82">
+        <f>PEARSON(K77:K80,L77:L80)</f>
+        <v>-5.7798604299139106E-2</v>
+      </c>
+      <c r="N82">
+        <f>PEARSON(M77:M80,N77:N80)</f>
+        <v>-0.99992673890923056</v>
+      </c>
+      <c r="P82">
+        <f>PEARSON(O77:O80,P77:P80)</f>
+        <v>0.62403125607886034</v>
+      </c>
+      <c r="R82">
+        <f>PEARSON(Q77:Q80,R77:R80)</f>
+        <v>-0.92852390618539415</v>
+      </c>
+      <c r="T82">
+        <f>PEARSON(S77:S80,T77:T80)</f>
+        <v>-0.91891346965103771</v>
+      </c>
+      <c r="V82">
+        <f>PEARSON(U77:U80,V77:V80)</f>
+        <v>0.77458568297423736</v>
+      </c>
+      <c r="X82">
+        <f>PEARSON(W77:W80,X77:X80)</f>
+        <v>-0.63901416506036224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>